<commit_message>
Adding invalid login test cases
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Selenium_B66\pk-hybridframework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CDE1E4-33E4-4A48-ACC4-9B83135E416F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A74D71-C295-4042-BCB4-ED1D96AE69EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcase1" sheetId="1" r:id="rId1"/>
+    <sheet name="VerifyActiTimeLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +26,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>Pawan</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>pawan</t>
   </si>
 </sst>
 </file>
@@ -350,7 +366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -369,4 +385,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA0D0B0-08D1-47C3-977A-3A18A3F8D5B4}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>